<commit_message>
Updated the users and fixtures list
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -565,8 +565,12 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -602,8 +606,12 @@
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -639,8 +647,12 @@
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -676,8 +688,12 @@
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -713,8 +729,12 @@
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -750,8 +770,12 @@
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">

</xml_diff>

<commit_message>
Updated the user and fixture data
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -811,8 +811,12 @@
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>3</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">

</xml_diff>

<commit_message>
Updated users and fixtures, added view for submitted predictions
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -1057,8 +1057,12 @@
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1094,8 +1098,12 @@
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1131,8 +1139,12 @@
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1168,8 +1180,12 @@
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1205,8 +1221,12 @@
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">

</xml_diff>

<commit_message>
Updated users and fixtures list
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -852,8 +852,12 @@
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -889,8 +893,12 @@
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -926,8 +934,12 @@
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -963,8 +975,12 @@
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1000,8 +1016,12 @@
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1037,8 +1057,12 @@
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1074,8 +1098,12 @@
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1111,8 +1139,12 @@
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1148,8 +1180,12 @@
         </is>
       </c>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1185,8 +1221,12 @@
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">

</xml_diff>

<commit_message>
Updated the users list and fixtures list with new fixtures
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -5,45 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\exportData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\eventData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240D24F8-BF87-40BB-BA11-EC9235807555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F4E9E-8F3A-4689-8B49-A95B56438141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31680" yWindow="900" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="UNI_AA_VERSION" hidden="1">"323.1.0"</definedName>
-    <definedName name="UNI_PRES_CLOSEST" hidden="1">512</definedName>
-    <definedName name="UNI_PRES_FILTER" hidden="1">1</definedName>
-    <definedName name="UNI_PRES_HEADINGS" hidden="1">16</definedName>
-    <definedName name="UNI_PRES_INVERT" hidden="1">2</definedName>
-    <definedName name="UNI_PRES_MATRIX" hidden="1">4</definedName>
-    <definedName name="UNI_PRES_MERGED" hidden="1">8</definedName>
-    <definedName name="UNI_PRES_MRECORD" hidden="1">64</definedName>
-    <definedName name="UNI_PRES_MSTIME" hidden="1">8192</definedName>
-    <definedName name="UNI_PRES_POST" hidden="1">256</definedName>
-    <definedName name="UNI_PRES_PRIOR" hidden="1">2048</definedName>
-    <definedName name="UNI_PRES_RECENT" hidden="1">1024</definedName>
-    <definedName name="UNI_PRES_STATIC" hidden="1">128</definedName>
-    <definedName name="UNI_PRES_TRANSPOSE" hidden="1">4096</definedName>
-    <definedName name="UNI_RET_ATTRIB" hidden="1">64</definedName>
-    <definedName name="UNI_RET_CONF" hidden="1">32</definedName>
-    <definedName name="UNI_RET_DESC" hidden="1">4</definedName>
-    <definedName name="UNI_RET_TAG" hidden="1">1</definedName>
-    <definedName name="UNI_RET_TIME" hidden="1">8</definedName>
-    <definedName name="UNI_RET_UNIT" hidden="1">2</definedName>
-    <definedName name="UNI_RET_VALUE" hidden="1">16</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="74">
   <si>
     <t>Day</t>
   </si>
@@ -259,6 +236,12 @@
   </si>
   <si>
     <t>Jul 02, 2024</t>
+  </si>
+  <si>
+    <t>Jul 05, 2024</t>
+  </si>
+  <si>
+    <t>Jul 06, 2024</t>
   </si>
 </sst>
 </file>
@@ -627,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,6 +1608,12 @@
       <c r="H38" t="s">
         <v>26</v>
       </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1645,6 +1634,12 @@
       <c r="H39" t="s">
         <v>29</v>
       </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1665,6 +1660,12 @@
       <c r="H40" t="s">
         <v>40</v>
       </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1685,6 +1686,12 @@
       <c r="H41" t="s">
         <v>22</v>
       </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1705,6 +1712,12 @@
       <c r="H42" t="s">
         <v>50</v>
       </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1725,6 +1738,12 @@
       <c r="H43" t="s">
         <v>47</v>
       </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1745,6 +1764,12 @@
       <c r="H44" t="s">
         <v>16</v>
       </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1764,6 +1789,92 @@
       </c>
       <c r="H45" t="s">
         <v>57</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" t="s">
+        <v>53</v>
+      </c>
+      <c r="H49" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added updated user and fixture list
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -5,45 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\exportData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\eventData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240D24F8-BF87-40BB-BA11-EC9235807555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F4E9E-8F3A-4689-8B49-A95B56438141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31680" yWindow="900" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="UNI_AA_VERSION" hidden="1">"323.1.0"</definedName>
-    <definedName name="UNI_PRES_CLOSEST" hidden="1">512</definedName>
-    <definedName name="UNI_PRES_FILTER" hidden="1">1</definedName>
-    <definedName name="UNI_PRES_HEADINGS" hidden="1">16</definedName>
-    <definedName name="UNI_PRES_INVERT" hidden="1">2</definedName>
-    <definedName name="UNI_PRES_MATRIX" hidden="1">4</definedName>
-    <definedName name="UNI_PRES_MERGED" hidden="1">8</definedName>
-    <definedName name="UNI_PRES_MRECORD" hidden="1">64</definedName>
-    <definedName name="UNI_PRES_MSTIME" hidden="1">8192</definedName>
-    <definedName name="UNI_PRES_POST" hidden="1">256</definedName>
-    <definedName name="UNI_PRES_PRIOR" hidden="1">2048</definedName>
-    <definedName name="UNI_PRES_RECENT" hidden="1">1024</definedName>
-    <definedName name="UNI_PRES_STATIC" hidden="1">128</definedName>
-    <definedName name="UNI_PRES_TRANSPOSE" hidden="1">4096</definedName>
-    <definedName name="UNI_RET_ATTRIB" hidden="1">64</definedName>
-    <definedName name="UNI_RET_CONF" hidden="1">32</definedName>
-    <definedName name="UNI_RET_DESC" hidden="1">4</definedName>
-    <definedName name="UNI_RET_TAG" hidden="1">1</definedName>
-    <definedName name="UNI_RET_TIME" hidden="1">8</definedName>
-    <definedName name="UNI_RET_UNIT" hidden="1">2</definedName>
-    <definedName name="UNI_RET_VALUE" hidden="1">16</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="74">
   <si>
     <t>Day</t>
   </si>
@@ -259,6 +236,12 @@
   </si>
   <si>
     <t>Jul 02, 2024</t>
+  </si>
+  <si>
+    <t>Jul 05, 2024</t>
+  </si>
+  <si>
+    <t>Jul 06, 2024</t>
   </si>
 </sst>
 </file>
@@ -627,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,6 +1608,12 @@
       <c r="H38" t="s">
         <v>26</v>
       </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1645,6 +1634,12 @@
       <c r="H39" t="s">
         <v>29</v>
       </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1665,6 +1660,12 @@
       <c r="H40" t="s">
         <v>40</v>
       </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1685,6 +1686,12 @@
       <c r="H41" t="s">
         <v>22</v>
       </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1705,6 +1712,12 @@
       <c r="H42" t="s">
         <v>50</v>
       </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1725,6 +1738,12 @@
       <c r="H43" t="s">
         <v>47</v>
       </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1745,6 +1764,12 @@
       <c r="H44" t="s">
         <v>16</v>
       </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1764,6 +1789,92 @@
       </c>
       <c r="H45" t="s">
         <v>57</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" t="s">
+        <v>53</v>
+      </c>
+      <c r="H49" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update users and fixtures list
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\eventData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oxp02030\Downloads\ineos-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F4E9E-8F3A-4689-8B49-A95B56438141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB82FE-246E-476C-857C-85B3192C270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="76">
   <si>
     <t>Day</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Jul 06, 2024</t>
+  </si>
+  <si>
+    <t>Jul 09, 2024</t>
+  </si>
+  <si>
+    <t>Jul 10, 2024</t>
   </si>
 </sst>
 </file>
@@ -610,13 +616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1816,6 +1825,12 @@
       <c r="H46" t="s">
         <v>37</v>
       </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1836,6 +1851,12 @@
       <c r="H47" t="s">
         <v>34</v>
       </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1856,8 +1877,14 @@
       <c r="H48" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1875,6 +1902,52 @@
       </c>
       <c r="H49" t="s">
         <v>26</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" t="s">
+        <v>39</v>
+      </c>
+      <c r="H51" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the users and fixture list
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\EuroPredictorGame-streamlit\eventData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oxp02030\Downloads\ineos-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F4E9E-8F3A-4689-8B49-A95B56438141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB82FE-246E-476C-857C-85B3192C270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="76">
   <si>
     <t>Day</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Jul 06, 2024</t>
+  </si>
+  <si>
+    <t>Jul 09, 2024</t>
+  </si>
+  <si>
+    <t>Jul 10, 2024</t>
   </si>
 </sst>
 </file>
@@ -610,13 +616,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1816,6 +1825,12 @@
       <c r="H46" t="s">
         <v>37</v>
       </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1836,6 +1851,12 @@
       <c r="H47" t="s">
         <v>34</v>
       </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1856,8 +1877,14 @@
       <c r="H48" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1875,6 +1902,52 @@
       </c>
       <c r="H49" t="s">
         <v>26</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
+        <v>24</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" t="s">
+        <v>39</v>
+      </c>
+      <c r="H51" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated users and fixture list
</commit_message>
<xml_diff>
--- a/eventData/fixture list.xlsx
+++ b/eventData/fixture list.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oxp02030\Downloads\ineos-game\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CB82FE-246E-476C-857C-85B3192C270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{0B82DF53-BE7C-F745-953E-1C261573944C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="76">
   <si>
     <t>Day</t>
   </si>
@@ -254,7 +262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,12 +274,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,11 +311,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,18 +619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -688,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -714,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -766,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -792,7 +792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -844,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -870,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -896,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -922,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -948,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -974,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1929,8 +1929,14 @@
       <c r="H50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1949,9 +1955,34 @@
       <c r="H51" t="s">
         <v>29</v>
       </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="2">
+        <v>45487</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>